<commit_message>
change in data (some measurements)
</commit_message>
<xml_diff>
--- a/analysis_all.cycles/derived_data/AvsN_all.cycles.xlsx
+++ b/analysis_all.cycles/derived_data/AvsN_all.cycles.xlsx
@@ -162,10 +162,10 @@
     <t xml:space="preserve">8/10/2021 7:41:36 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">2021/10/22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12:03:02</t>
+    <t xml:space="preserve">2022/10/04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15:56:47</t>
   </si>
   <si>
     <t xml:space="preserve">B</t>
@@ -174,7 +174,7 @@
     <t xml:space="preserve">8/10/2021 7:59:13 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:03:14</t>
+    <t xml:space="preserve">15:56:59</t>
   </si>
   <si>
     <t xml:space="preserve">C</t>
@@ -183,7 +183,7 @@
     <t xml:space="preserve">8/10/2021 8:14:18 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:03:25</t>
+    <t xml:space="preserve">15:57:11</t>
   </si>
   <si>
     <t xml:space="preserve">1000</t>
@@ -192,19 +192,19 @@
     <t xml:space="preserve">10/12/2021 8:36:04 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:03:38</t>
+    <t xml:space="preserve">15:57:25</t>
   </si>
   <si>
     <t xml:space="preserve">10/12/2021 9:21:30 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:03:50</t>
+    <t xml:space="preserve">15:57:36</t>
   </si>
   <si>
     <t xml:space="preserve">10/12/2021 10:22:07 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:04:01</t>
+    <t xml:space="preserve">15:57:47</t>
   </si>
   <si>
     <t xml:space="preserve">2000</t>
@@ -213,19 +213,19 @@
     <t xml:space="preserve">8/9/2021 10:10:48 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:04:15</t>
+    <t xml:space="preserve">15:58:00</t>
   </si>
   <si>
     <t xml:space="preserve">8/9/2021 12:13:28 PM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:04:28</t>
+    <t xml:space="preserve">15:58:12</t>
   </si>
   <si>
     <t xml:space="preserve">8/9/2021 1:26:13 PM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:04:40</t>
+    <t xml:space="preserve">15:58:22</t>
   </si>
   <si>
     <t xml:space="preserve">250</t>
@@ -234,19 +234,19 @@
     <t xml:space="preserve">10/11/2021 8:34:41 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:04:54</t>
+    <t xml:space="preserve">15:58:35</t>
   </si>
   <si>
     <t xml:space="preserve">10/11/2021 8:50:40 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:05:07</t>
+    <t xml:space="preserve">15:58:47</t>
   </si>
   <si>
     <t xml:space="preserve">10/11/2021 9:05:03 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:05:19</t>
+    <t xml:space="preserve">15:58:58</t>
   </si>
   <si>
     <t xml:space="preserve">50</t>
@@ -255,19 +255,19 @@
     <t xml:space="preserve">10/5/2021 9:52:32 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:05:33</t>
+    <t xml:space="preserve">15:59:13</t>
   </si>
   <si>
     <t xml:space="preserve">10/5/2021 11:18:53 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:05:45</t>
+    <t xml:space="preserve">15:59:25</t>
   </si>
   <si>
     <t xml:space="preserve">10/5/2021 11:39:21 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:05:55</t>
+    <t xml:space="preserve">15:59:36</t>
   </si>
   <si>
     <t xml:space="preserve">FLT4-15</t>
@@ -279,88 +279,88 @@
     <t xml:space="preserve">8/4/2021 12:01:54 PM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:06:09</t>
+    <t xml:space="preserve">15:59:50</t>
   </si>
   <si>
     <t xml:space="preserve">8/4/2021 12:14:56 PM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:06:22</t>
+    <t xml:space="preserve">16:00:04</t>
   </si>
   <si>
     <t xml:space="preserve">8/4/2021 12:36:53 PM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:06:33</t>
+    <t xml:space="preserve">16:00:16</t>
   </si>
   <si>
     <t xml:space="preserve">10/12/2021 11:41:56 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:06:47</t>
+    <t xml:space="preserve">16:00:31</t>
   </si>
   <si>
     <t xml:space="preserve">10/12/2021 12:15:25 PM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:07:00</t>
+    <t xml:space="preserve">16:00:45</t>
   </si>
   <si>
     <t xml:space="preserve">10/12/2021 1:12:47 PM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:07:11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8/4/2021 8:47:04 AM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12:07:25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8/4/2021 9:50:52 AM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12:07:39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8/4/2021 11:04:57 AM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12:07:50</t>
+    <t xml:space="preserve">16:00:57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9/28/2022 9:42:07 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16:01:11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9/28/2022 10:06:49 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16:01:24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9/28/2022 10:16:07 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16:01:37</t>
   </si>
   <si>
     <t xml:space="preserve">10/11/2021 9:31:49 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:08:03</t>
+    <t xml:space="preserve">16:01:51</t>
   </si>
   <si>
     <t xml:space="preserve">10/11/2021 9:52:56 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:08:17</t>
+    <t xml:space="preserve">16:02:05</t>
   </si>
   <si>
     <t xml:space="preserve">10/11/2021 11:03:18 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:08:27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12:08:41</t>
+    <t xml:space="preserve">16:02:16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16:02:29</t>
   </si>
   <si>
     <t xml:space="preserve">10/5/2021 8:57:35 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:08:54</t>
+    <t xml:space="preserve">16:02:42</t>
   </si>
   <si>
     <t xml:space="preserve">10/5/2021 9:20:52 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:09:05</t>
+    <t xml:space="preserve">16:02:53</t>
   </si>
   <si>
     <t xml:space="preserve">FLT4-7</t>
@@ -372,91 +372,91 @@
     <t xml:space="preserve">8/5/2021 10:37:26 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:09:18</t>
+    <t xml:space="preserve">16:03:06</t>
   </si>
   <si>
     <t xml:space="preserve">8/5/2021 11:29:25 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:09:32</t>
+    <t xml:space="preserve">16:03:20</t>
   </si>
   <si>
     <t xml:space="preserve">8/5/2021 12:04:56 PM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:09:47</t>
+    <t xml:space="preserve">16:03:34</t>
   </si>
   <si>
     <t xml:space="preserve">10/11/2021 12:49:58 PM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:10:02</t>
+    <t xml:space="preserve">16:03:48</t>
   </si>
   <si>
     <t xml:space="preserve">10/11/2021 1:38:03 PM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:10:17</t>
+    <t xml:space="preserve">16:04:01</t>
   </si>
   <si>
     <t xml:space="preserve">10/11/2021 2:25:04 PM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:10:31</t>
+    <t xml:space="preserve">16:04:15</t>
   </si>
   <si>
     <t xml:space="preserve">8/5/2021 8:53:28 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:10:45</t>
+    <t xml:space="preserve">16:04:28</t>
   </si>
   <si>
     <t xml:space="preserve">8/5/2021 9:04:53 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:10:58</t>
+    <t xml:space="preserve">16:04:41</t>
   </si>
   <si>
     <t xml:space="preserve">8/5/2021 9:21:43 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:11:12</t>
+    <t xml:space="preserve">16:04:54</t>
   </si>
   <si>
     <t xml:space="preserve">10/8/2021 11:34:58 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:11:26</t>
+    <t xml:space="preserve">16:05:08</t>
   </si>
   <si>
     <t xml:space="preserve">10/8/2021 11:59:48 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:11:40</t>
+    <t xml:space="preserve">16:05:21</t>
   </si>
   <si>
     <t xml:space="preserve">10/8/2021 12:19:29 PM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:11:54</t>
+    <t xml:space="preserve">16:05:34</t>
   </si>
   <si>
     <t xml:space="preserve">10/5/2021 12:26:59 PM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:12:08</t>
+    <t xml:space="preserve">16:05:48</t>
   </si>
   <si>
     <t xml:space="preserve">10/5/2021 2:20:51 PM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:12:22</t>
+    <t xml:space="preserve">16:06:01</t>
   </si>
   <si>
     <t xml:space="preserve">10/5/2021 1:33:21 PM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:12:36</t>
+    <t xml:space="preserve">16:06:14</t>
   </si>
   <si>
     <t xml:space="preserve">FLT4-8</t>
@@ -468,85 +468,85 @@
     <t xml:space="preserve">8/6/2021 10:32:31 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:12:50</t>
+    <t xml:space="preserve">16:06:27</t>
   </si>
   <si>
     <t xml:space="preserve">8/6/2021 11:21:08 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:13:03</t>
+    <t xml:space="preserve">16:06:41</t>
   </si>
   <si>
     <t xml:space="preserve">8/6/2021 11:45:42 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:13:16</t>
+    <t xml:space="preserve">16:06:53</t>
   </si>
   <si>
     <t xml:space="preserve">10/12/2021 7:28:58 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:13:30</t>
+    <t xml:space="preserve">16:07:06</t>
   </si>
   <si>
     <t xml:space="preserve">10/12/2021 7:46:04 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:13:43</t>
+    <t xml:space="preserve">16:07:18</t>
   </si>
   <si>
     <t xml:space="preserve">10/12/2021 8:02:39 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:13:56</t>
+    <t xml:space="preserve">16:07:31</t>
   </si>
   <si>
     <t xml:space="preserve">8/6/2021 9:27:47 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:14:09</t>
+    <t xml:space="preserve">16:07:43</t>
   </si>
   <si>
     <t xml:space="preserve">8/6/2021 9:41:49 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:14:21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12:14:33</t>
+    <t xml:space="preserve">16:07:55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16:08:08</t>
   </si>
   <si>
     <t xml:space="preserve">10/11/2021 7:35:06 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:14:46</t>
+    <t xml:space="preserve">16:08:20</t>
   </si>
   <si>
     <t xml:space="preserve">10/11/2021 7:50:09 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:14:58</t>
+    <t xml:space="preserve">16:08:33</t>
   </si>
   <si>
     <t xml:space="preserve">10/11/2021 8:08:19 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:15:09</t>
+    <t xml:space="preserve">16:08:44</t>
   </si>
   <si>
     <t xml:space="preserve">10/5/2021 2:06:34 PM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:15:22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12:15:36</t>
+    <t xml:space="preserve">16:08:57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16:09:09</t>
   </si>
   <si>
     <t xml:space="preserve">10/5/2021 2:37:13 PM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:15:48</t>
+    <t xml:space="preserve">16:09:21</t>
   </si>
   <si>
     <t xml:space="preserve">LYDIT4-11</t>
@@ -558,88 +558,88 @@
     <t xml:space="preserve">7/30/2021 12:28:40 PM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:16:01</t>
+    <t xml:space="preserve">16:09:34</t>
   </si>
   <si>
     <t xml:space="preserve">7/30/2021 12:42:08 PM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:16:14</t>
+    <t xml:space="preserve">16:09:47</t>
   </si>
   <si>
     <t xml:space="preserve">7/30/2021 1:08:52 PM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:16:27</t>
+    <t xml:space="preserve">16:10:00</t>
   </si>
   <si>
     <t xml:space="preserve">10/8/2021 7:33:17 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:16:40</t>
+    <t xml:space="preserve">16:10:13</t>
   </si>
   <si>
     <t xml:space="preserve">10/8/2021 7:47:19 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:16:54</t>
+    <t xml:space="preserve">16:10:26</t>
   </si>
   <si>
     <t xml:space="preserve">10/8/2021 8:02:34 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:17:07</t>
+    <t xml:space="preserve">16:10:39</t>
   </si>
   <si>
     <t xml:space="preserve">7/30/2021 10:47:48 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:17:20</t>
+    <t xml:space="preserve">16:10:52</t>
   </si>
   <si>
     <t xml:space="preserve">7/30/2021 11:45:07 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:17:33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12:17:46</t>
+    <t xml:space="preserve">16:11:05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16:11:18</t>
   </si>
   <si>
     <t xml:space="preserve">10/7/2021 7:49:19 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:18:00</t>
+    <t xml:space="preserve">16:11:32</t>
   </si>
   <si>
     <t xml:space="preserve">10/7/2021 8:06:29 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:18:13</t>
+    <t xml:space="preserve">16:11:45</t>
   </si>
   <si>
     <t xml:space="preserve">10/7/2021 8:23:48 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:18:26</t>
+    <t xml:space="preserve">16:11:59</t>
   </si>
   <si>
     <t xml:space="preserve">10/4/2021 1:49:45 PM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:18:40</t>
+    <t xml:space="preserve">16:12:12</t>
   </si>
   <si>
     <t xml:space="preserve">10/4/2021 2:03:49 PM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:18:53</t>
+    <t xml:space="preserve">16:12:25</t>
   </si>
   <si>
     <t xml:space="preserve">10/4/2021 2:16:58 PM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:19:06</t>
+    <t xml:space="preserve">16:12:38</t>
   </si>
   <si>
     <t xml:space="preserve">LYDIT4-1</t>
@@ -648,91 +648,91 @@
     <t xml:space="preserve">8/3/2021 9:18:21 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:19:19</t>
+    <t xml:space="preserve">16:12:51</t>
   </si>
   <si>
     <t xml:space="preserve">8/3/2021 9:43:36 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:19:32</t>
+    <t xml:space="preserve">16:13:04</t>
   </si>
   <si>
     <t xml:space="preserve">8/3/2021 10:07:30 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:19:41</t>
+    <t xml:space="preserve">16:13:12</t>
   </si>
   <si>
     <t xml:space="preserve">10/7/2021 8:58:14 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:19:53</t>
+    <t xml:space="preserve">16:13:25</t>
   </si>
   <si>
     <t xml:space="preserve">10/7/2021 9:17:38 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:20:06</t>
+    <t xml:space="preserve">16:13:37</t>
   </si>
   <si>
     <t xml:space="preserve">10/7/2021 9:35:01 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:20:14</t>
+    <t xml:space="preserve">16:13:45</t>
   </si>
   <si>
     <t xml:space="preserve">8/3/2021 8:01:53 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:20:26</t>
+    <t xml:space="preserve">16:13:58</t>
   </si>
   <si>
     <t xml:space="preserve">8/3/2021 8:13:56 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:20:39</t>
+    <t xml:space="preserve">16:14:10</t>
   </si>
   <si>
     <t xml:space="preserve">8/3/2021 8:39:33 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:20:47</t>
+    <t xml:space="preserve">16:14:18</t>
   </si>
   <si>
     <t xml:space="preserve">10/6/2021 7:38:21 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:21:00</t>
+    <t xml:space="preserve">16:14:31</t>
   </si>
   <si>
     <t xml:space="preserve">10/6/2021 8:02:05 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:21:13</t>
+    <t xml:space="preserve">16:14:43</t>
   </si>
   <si>
     <t xml:space="preserve">10/6/2021 8:23:57 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:21:21</t>
+    <t xml:space="preserve">16:14:51</t>
   </si>
   <si>
     <t xml:space="preserve">10/4/2021 2:43:06 PM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:21:35</t>
+    <t xml:space="preserve">16:15:05</t>
   </si>
   <si>
     <t xml:space="preserve">10/4/2021 3:09:07 PM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:21:48</t>
+    <t xml:space="preserve">16:15:18</t>
   </si>
   <si>
     <t xml:space="preserve">10/4/2021 3:40:26 PM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:21:57</t>
+    <t xml:space="preserve">16:15:27</t>
   </si>
   <si>
     <t xml:space="preserve">LYDIT4-2</t>
@@ -741,91 +741,91 @@
     <t xml:space="preserve">8/2/2021 2:20:02 PM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:22:10</t>
+    <t xml:space="preserve">16:15:40</t>
   </si>
   <si>
     <t xml:space="preserve">8/2/2021 1:59:29 PM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:22:24</t>
+    <t xml:space="preserve">16:15:54</t>
   </si>
   <si>
     <t xml:space="preserve">8/2/2021 2:36:43 PM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:22:37</t>
+    <t xml:space="preserve">16:16:07</t>
   </si>
   <si>
     <t xml:space="preserve">10/7/2021 10:34:37 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:22:51</t>
+    <t xml:space="preserve">16:16:21</t>
   </si>
   <si>
     <t xml:space="preserve">10/7/2021 11:32:10 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:23:05</t>
+    <t xml:space="preserve">16:16:34</t>
   </si>
   <si>
     <t xml:space="preserve">10/7/2021 12:32:49 PM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:23:19</t>
+    <t xml:space="preserve">16:16:48</t>
   </si>
   <si>
     <t xml:space="preserve">8/2/2021 11:06:08 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:23:32</t>
+    <t xml:space="preserve">16:17:01</t>
   </si>
   <si>
     <t xml:space="preserve">8/2/2021 11:55:00 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:23:46</t>
+    <t xml:space="preserve">16:17:15</t>
   </si>
   <si>
     <t xml:space="preserve">8/2/2021 1:18:04 PM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:23:59</t>
+    <t xml:space="preserve">16:17:28</t>
   </si>
   <si>
     <t xml:space="preserve">10/6/2021 10:19:27 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:24:13</t>
+    <t xml:space="preserve">16:17:42</t>
   </si>
   <si>
     <t xml:space="preserve">10/8/2021 9:48:39 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:24:27</t>
+    <t xml:space="preserve">16:17:56</t>
   </si>
   <si>
     <t xml:space="preserve">10/8/2021 10:32:29 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:24:40</t>
+    <t xml:space="preserve">16:18:10</t>
   </si>
   <si>
     <t xml:space="preserve">10/5/2021 7:37:44 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:24:54</t>
+    <t xml:space="preserve">16:18:23</t>
   </si>
   <si>
     <t xml:space="preserve">10/5/2021 7:48:49 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:25:07</t>
+    <t xml:space="preserve">16:18:36</t>
   </si>
   <si>
     <t xml:space="preserve">10/5/2021 8:00:26 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:25:21</t>
+    <t xml:space="preserve">16:18:49</t>
   </si>
   <si>
     <t xml:space="preserve">LYDIT4-7</t>
@@ -834,88 +834,88 @@
     <t xml:space="preserve">7/26/2021 10:05:58 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:25:34</t>
+    <t xml:space="preserve">16:19:02</t>
   </si>
   <si>
     <t xml:space="preserve">7/26/2021 10:23:26 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:25:48</t>
+    <t xml:space="preserve">16:19:15</t>
   </si>
   <si>
     <t xml:space="preserve">7/26/2021 10:44:32 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:26:02</t>
+    <t xml:space="preserve">16:19:29</t>
   </si>
   <si>
     <t xml:space="preserve">10/7/2021 2:07:58 PM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:26:16</t>
+    <t xml:space="preserve">16:19:42</t>
   </si>
   <si>
     <t xml:space="preserve">10/7/2021 2:28:03 PM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:26:30</t>
+    <t xml:space="preserve">16:19:55</t>
   </si>
   <si>
     <t xml:space="preserve">10/7/2021 2:46:53 PM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:26:43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7/23/2021 8:41:54 AM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12:26:57</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7/23/2021 9:25:44 AM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12:27:10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7/23/2021 11:33:58 AM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12:27:23</t>
+    <t xml:space="preserve">16:20:08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9/27/2022 10:23:39 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16:20:21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9/27/2022 10:43:51 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16:20:34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9/27/2022 11:36:41 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16:20:46</t>
   </si>
   <si>
     <t xml:space="preserve">10/4/2021 12:12:16 PM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:27:36</t>
+    <t xml:space="preserve">16:21:02</t>
   </si>
   <si>
     <t xml:space="preserve">10/6/2021 1:29:51 PM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:27:50</t>
+    <t xml:space="preserve">16:21:17</t>
   </si>
   <si>
     <t xml:space="preserve">10/6/2021 2:14:10 PM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:28:04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12:28:17</t>
+    <t xml:space="preserve">16:21:32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16:21:46</t>
   </si>
   <si>
     <t xml:space="preserve">10/4/2021 12:35:02 PM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:28:31</t>
+    <t xml:space="preserve">16:21:59</t>
   </si>
   <si>
     <t xml:space="preserve">10/4/2021 12:51:39 PM</t>
   </si>
   <si>
-    <t xml:space="preserve">12:28:44</t>
+    <t xml:space="preserve">16:22:13</t>
   </si>
   <si>
     <t xml:space="preserve">variable</t>
@@ -4276,109 +4276,105 @@
         <v>100</v>
       </c>
       <c r="I23" t="n">
-        <v>4501.009431</v>
+        <v>3356.384132</v>
       </c>
       <c r="J23" t="n">
-        <v>0.524531197</v>
+        <v>0.4405003237</v>
       </c>
       <c r="K23" t="n">
-        <v>6.969785641</v>
+        <v>7.149735069</v>
       </c>
       <c r="L23" t="n">
-        <v>23534.20402</v>
+        <v>15591.80448</v>
       </c>
       <c r="M23" t="n">
-        <v>16623.99631</v>
+        <v>11634.05861</v>
       </c>
       <c r="N23" t="n">
-        <v>40158.20034</v>
+        <v>27225.86308</v>
       </c>
       <c r="O23" t="n">
-        <v>2988.772723</v>
+        <v>2276.246374</v>
       </c>
       <c r="P23" t="n">
-        <v>0.05465177769</v>
+        <v>0.3530863765</v>
       </c>
       <c r="Q23" t="n">
-        <v>3519.476967</v>
+        <v>3048.436614</v>
       </c>
       <c r="R23" t="n">
-        <v>9871.137458</v>
+        <v>8036.763981</v>
       </c>
       <c r="S23" t="n">
-        <v>17.39910022</v>
-      </c>
-      <c r="T23" t="n">
-        <v>0.1645345816</v>
-      </c>
+        <v>19.89117331</v>
+      </c>
+      <c r="T23"/>
       <c r="U23" t="n">
-        <v>137.5071312</v>
+        <v>137.0104181</v>
       </c>
       <c r="V23" t="n">
-        <v>0.6954043106</v>
+        <v>0.5849291009</v>
       </c>
       <c r="W23" t="n">
-        <v>9.052066888</v>
+        <v>6.684481704</v>
       </c>
       <c r="X23" t="n">
-        <v>0.5119881142</v>
+        <v>0.3070656808</v>
       </c>
       <c r="Y23" t="n">
-        <v>4.031475464</v>
+        <v>3.355539105</v>
       </c>
       <c r="Z23" t="n">
-        <v>0.5119881142</v>
+        <v>0.3070656808</v>
       </c>
       <c r="AA23" t="n">
-        <v>2.478067839</v>
+        <v>1.969662632</v>
       </c>
       <c r="AB23" t="n">
-        <v>3.306943218</v>
+        <v>2.848009221</v>
       </c>
       <c r="AC23" t="n">
-        <v>0.7245322461</v>
+        <v>0.5075298843</v>
       </c>
       <c r="AD23" t="n">
-        <v>19352.38225</v>
+        <v>12483.33768</v>
       </c>
       <c r="AE23" t="n">
-        <v>2094.470119</v>
+        <v>1105.887442</v>
       </c>
       <c r="AF23" t="n">
-        <v>2480.200412</v>
-      </c>
-      <c r="AG23" t="n">
-        <v>16.45345816</v>
-      </c>
+        <v>2968.976909</v>
+      </c>
+      <c r="AG23"/>
       <c r="AH23" t="n">
-        <v>135.3093971</v>
+        <v>134.4816023</v>
       </c>
       <c r="AI23" t="n">
-        <v>141.45912</v>
+        <v>90.03655912</v>
       </c>
       <c r="AJ23" t="n">
-        <v>153.4881304</v>
+        <v>153.0178095</v>
       </c>
       <c r="AK23" t="n">
-        <v>10.30486308</v>
+        <v>11.96122982</v>
       </c>
       <c r="AL23" t="n">
-        <v>0.004847845905</v>
+        <v>0.003897660015</v>
       </c>
       <c r="AM23" t="n">
-        <v>0.01780910934</v>
+        <v>0.01621683835</v>
       </c>
       <c r="AN23" t="n">
-        <v>12.90435761</v>
+        <v>9.860444899</v>
       </c>
       <c r="AO23" t="n">
-        <v>472.6900437</v>
+        <v>194.2276601</v>
       </c>
       <c r="AP23" t="n">
-        <v>17.38212743</v>
+        <v>20.64856518</v>
       </c>
       <c r="AQ23" t="n">
-        <v>7.726904954</v>
+        <v>7.772076185</v>
       </c>
     </row>
     <row r="24">
@@ -4407,109 +4403,109 @@
         <v>102</v>
       </c>
       <c r="I24" t="n">
-        <v>7193.848092</v>
+        <v>221.8181278</v>
       </c>
       <c r="J24" t="n">
-        <v>-0.3689415062</v>
+        <v>1.783246621</v>
       </c>
       <c r="K24" t="n">
-        <v>7.636845113</v>
+        <v>9.26438122</v>
       </c>
       <c r="L24" t="n">
-        <v>41460.209</v>
+        <v>1413.323285</v>
       </c>
       <c r="M24" t="n">
-        <v>35011.89307</v>
+        <v>523.459649</v>
       </c>
       <c r="N24" t="n">
-        <v>76472.10206</v>
+        <v>1936.782934</v>
       </c>
       <c r="O24" t="n">
-        <v>5299.129728</v>
+        <v>154.6577046</v>
       </c>
       <c r="P24" t="n">
-        <v>0.1018678189</v>
+        <v>4.456298992</v>
       </c>
       <c r="Q24" t="n">
-        <v>7354.654409</v>
+        <v>237.3281076</v>
       </c>
       <c r="R24" t="n">
-        <v>15021.89575</v>
+        <v>300.3844066</v>
       </c>
       <c r="S24" t="n">
-        <v>15.3537069</v>
+        <v>11.88111263</v>
       </c>
       <c r="T24" t="n">
-        <v>0.2300560506</v>
+        <v>0.7219131283</v>
       </c>
       <c r="U24" t="n">
-        <v>167.2473836</v>
+        <v>140.2547825</v>
       </c>
       <c r="V24" t="n">
-        <v>1.373777702</v>
+        <v>0.1286192565</v>
       </c>
       <c r="W24" t="n">
-        <v>37.40959111</v>
+        <v>0.8160222152</v>
       </c>
       <c r="X24" t="n">
-        <v>0.4053960358</v>
+        <v>0.02413911504</v>
       </c>
       <c r="Y24" t="n">
-        <v>7.760195161</v>
+        <v>0.2614672973</v>
       </c>
       <c r="Z24" t="n">
-        <v>0.4053960358</v>
+        <v>0.02413911504</v>
       </c>
       <c r="AA24" t="n">
-        <v>5.488816379</v>
+        <v>0.1514516566</v>
       </c>
       <c r="AB24" t="n">
-        <v>6.804879637</v>
+        <v>0.2444719719</v>
       </c>
       <c r="AC24" t="n">
-        <v>0.9553155241</v>
+        <v>0.01699532541</v>
       </c>
       <c r="AD24" t="n">
-        <v>36468.41961</v>
+        <v>918.1700024</v>
       </c>
       <c r="AE24" t="n">
-        <v>5678.854252</v>
+        <v>372.3052869</v>
       </c>
       <c r="AF24" t="n">
-        <v>2154.642922</v>
+        <v>3489.500156</v>
       </c>
       <c r="AG24" t="n">
-        <v>23.00560506</v>
+        <v>72.19131283</v>
       </c>
       <c r="AH24" t="n">
-        <v>179.9856311</v>
+        <v>89.97797456</v>
       </c>
       <c r="AI24" t="n">
-        <v>153.2612103</v>
+        <v>134.5306148</v>
       </c>
       <c r="AJ24" t="n">
-        <v>89.99714988</v>
+        <v>45.51840248</v>
       </c>
       <c r="AK24" t="n">
-        <v>10.54341589</v>
+        <v>88.77904999</v>
       </c>
       <c r="AL24" t="n">
-        <v>0.007092872671</v>
+        <v>0.0006089099577</v>
       </c>
       <c r="AM24" t="n">
-        <v>0.0207973236</v>
+        <v>0.01744344321</v>
       </c>
       <c r="AN24" t="n">
-        <v>54.06261393</v>
+        <v>1.795755289</v>
       </c>
       <c r="AO24" t="n">
-        <v>114.194612</v>
+        <v>2.900022818</v>
       </c>
       <c r="AP24" t="n">
-        <v>4.980027562</v>
+        <v>0.1712826421</v>
       </c>
       <c r="AQ24" t="n">
-        <v>5.354876555</v>
+        <v>0.2952172517</v>
       </c>
     </row>
     <row r="25">
@@ -4538,109 +4534,109 @@
         <v>104</v>
       </c>
       <c r="I25" t="n">
-        <v>294.7063455</v>
+        <v>361.4056273</v>
       </c>
       <c r="J25" t="n">
-        <v>1.489968377</v>
+        <v>2.73045764</v>
       </c>
       <c r="K25" t="n">
-        <v>9.129091947</v>
+        <v>15.84613941</v>
       </c>
       <c r="L25" t="n">
-        <v>1712.086538</v>
+        <v>3071.945338</v>
       </c>
       <c r="M25" t="n">
-        <v>1098.499087</v>
+        <v>736.2891459</v>
       </c>
       <c r="N25" t="n">
-        <v>2810.585624</v>
+        <v>3808.234484</v>
       </c>
       <c r="O25" t="n">
-        <v>194.6330773</v>
+        <v>236.5405273</v>
       </c>
       <c r="P25" t="n">
-        <v>3.194535635</v>
+        <v>0.367876445</v>
       </c>
       <c r="Q25" t="n">
-        <v>291.4904849</v>
+        <v>357.9118612</v>
       </c>
       <c r="R25" t="n">
-        <v>415.9483114</v>
+        <v>371.4418908</v>
       </c>
       <c r="S25" t="n">
-        <v>7.561461705</v>
+        <v>15.84721621</v>
       </c>
       <c r="T25" t="n">
-        <v>0.4795413196</v>
+        <v>0.6833324071</v>
       </c>
       <c r="U25" t="n">
-        <v>3.243347755</v>
+        <v>140.9960673</v>
       </c>
       <c r="V25" t="n">
-        <v>0.1312007135</v>
+        <v>0.1478422584</v>
       </c>
       <c r="W25" t="n">
-        <v>0.8436083717</v>
+        <v>1.06667361</v>
       </c>
       <c r="X25" t="n">
-        <v>0.03421041812</v>
+        <v>0.04485307824</v>
       </c>
       <c r="Y25" t="n">
-        <v>0.3256922005</v>
+        <v>0.4027685702</v>
       </c>
       <c r="Z25" t="n">
-        <v>0.03421041812</v>
+        <v>0.04485307824</v>
       </c>
       <c r="AA25" t="n">
-        <v>0.1767697105</v>
+        <v>0.2130352798</v>
       </c>
       <c r="AB25" t="n">
-        <v>0.2974636963</v>
+        <v>0.3823187992</v>
       </c>
       <c r="AC25" t="n">
-        <v>0.02822850418</v>
+        <v>0.02044977101</v>
       </c>
       <c r="AD25" t="n">
-        <v>1003.415011</v>
+        <v>1265.420975</v>
       </c>
       <c r="AE25" t="n">
-        <v>391.4424375</v>
+        <v>515.3623923</v>
       </c>
       <c r="AF25" t="n">
-        <v>3705.826963</v>
+        <v>3125.656529</v>
       </c>
       <c r="AG25" t="n">
-        <v>47.95413196</v>
+        <v>68.33324071</v>
       </c>
       <c r="AH25" t="n">
-        <v>179.9904511</v>
+        <v>44.99184546</v>
       </c>
       <c r="AI25" t="n">
-        <v>143.9993917</v>
+        <v>134.997763</v>
       </c>
       <c r="AJ25" t="n">
-        <v>124.4760875</v>
+        <v>179.9830999</v>
       </c>
       <c r="AK25" t="n">
-        <v>41.37489785</v>
+        <v>88.32116255</v>
       </c>
       <c r="AL25" t="n">
-        <v>0.002699521162</v>
+        <v>0.0001553256219</v>
       </c>
       <c r="AM25" t="n">
-        <v>0.0187792858</v>
+        <v>0.01760646407</v>
       </c>
       <c r="AN25" t="n">
-        <v>1.624680383</v>
+        <v>2.148273592</v>
       </c>
       <c r="AO25" t="n">
-        <v>4.504973664</v>
+        <v>3.06375382</v>
       </c>
       <c r="AP25" t="n">
-        <v>0.4429349619</v>
+        <v>0.1473286268</v>
       </c>
       <c r="AQ25" t="n">
-        <v>0.7960207451</v>
+        <v>0.3202782977</v>
       </c>
     </row>
     <row r="26">
@@ -16020,109 +16016,109 @@
         <v>285</v>
       </c>
       <c r="I113" t="n">
-        <v>2269.831713</v>
+        <v>1393.268784</v>
       </c>
       <c r="J113" t="n">
-        <v>1.786913422</v>
+        <v>0.956541288</v>
       </c>
       <c r="K113" t="n">
-        <v>9.640278553</v>
+        <v>4.72517791</v>
       </c>
       <c r="L113" t="n">
-        <v>13394.63384</v>
+        <v>6759.289134</v>
       </c>
       <c r="M113" t="n">
-        <v>5815.305195</v>
+        <v>3142.710302</v>
       </c>
       <c r="N113" t="n">
-        <v>19209.93903</v>
+        <v>9901.999436</v>
       </c>
       <c r="O113" t="n">
-        <v>1516.969116</v>
+        <v>1037.641018</v>
       </c>
       <c r="P113" t="n">
-        <v>0.2838102228</v>
+        <v>0.2182874011</v>
       </c>
       <c r="Q113" t="n">
-        <v>2205.090834</v>
+        <v>1755.782834</v>
       </c>
       <c r="R113" t="n">
-        <v>3516.905064</v>
+        <v>2121.325348</v>
       </c>
       <c r="S113" t="n">
-        <v>19.54294773</v>
+        <v>12.00231233</v>
       </c>
       <c r="T113" t="n">
-        <v>0.6562190201</v>
+        <v>0.4051772567</v>
       </c>
       <c r="U113" t="n">
-        <v>3.738615388</v>
+        <v>3.740178556</v>
       </c>
       <c r="V113" t="n">
-        <v>0.3404775841</v>
+        <v>0.3570209071</v>
       </c>
       <c r="W113" t="n">
-        <v>5.054978991</v>
+        <v>5.703690705</v>
       </c>
       <c r="X113" t="n">
-        <v>0.2701418412</v>
+        <v>0.1193322855</v>
       </c>
       <c r="Y113" t="n">
-        <v>2.47524455</v>
+        <v>1.875101789</v>
       </c>
       <c r="Z113" t="n">
-        <v>0.2701418412</v>
+        <v>0.1193322855</v>
       </c>
       <c r="AA113" t="n">
-        <v>1.43291113</v>
+        <v>1.101440313</v>
       </c>
       <c r="AB113" t="n">
-        <v>2.276327206</v>
+        <v>1.758522511</v>
       </c>
       <c r="AC113" t="n">
-        <v>0.1989173437</v>
+        <v>0.1165792784</v>
       </c>
       <c r="AD113" t="n">
-        <v>8334.500059</v>
+        <v>5021.221264</v>
       </c>
       <c r="AE113" t="n">
-        <v>2285.996372</v>
+        <v>1827.116345</v>
       </c>
       <c r="AF113" t="n">
-        <v>2021.702888</v>
+        <v>2664.102771</v>
       </c>
       <c r="AG113" t="n">
-        <v>65.62190201</v>
+        <v>40.51772567</v>
       </c>
       <c r="AH113" t="n">
-        <v>179.976296</v>
+        <v>0.003102536998</v>
       </c>
       <c r="AI113" t="n">
-        <v>45.04611176</v>
+        <v>90.01295815</v>
       </c>
       <c r="AJ113" t="n">
-        <v>153.5142623</v>
+        <v>116.4957164</v>
       </c>
       <c r="AK113" t="n">
-        <v>82.55169754</v>
+        <v>74.5552317</v>
       </c>
       <c r="AL113" t="n">
-        <v>0.002380658858</v>
+        <v>0.002476238483</v>
       </c>
       <c r="AM113" t="n">
-        <v>0.01813145204</v>
+        <v>0.01856849211</v>
       </c>
       <c r="AN113" t="n">
-        <v>7.025479077</v>
+        <v>9.740588409</v>
       </c>
       <c r="AO113" t="n">
-        <v>65.87096295</v>
+        <v>8.079234381</v>
       </c>
       <c r="AP113" t="n">
-        <v>0.3855007715</v>
+        <v>0.50664772</v>
       </c>
       <c r="AQ113" t="n">
-        <v>0.9496421854</v>
+        <v>0.7118703935</v>
       </c>
     </row>
     <row r="114">
@@ -16151,109 +16147,109 @@
         <v>287</v>
       </c>
       <c r="I114" t="n">
-        <v>3014.073384</v>
+        <v>1461.516107</v>
       </c>
       <c r="J114" t="n">
-        <v>1.228765154</v>
+        <v>1.478002772</v>
       </c>
       <c r="K114" t="n">
-        <v>7.136543031</v>
+        <v>7.265580345</v>
       </c>
       <c r="L114" t="n">
-        <v>16061.48819</v>
+        <v>8258.953213</v>
       </c>
       <c r="M114" t="n">
-        <v>8235.640915</v>
+        <v>3485.87432</v>
       </c>
       <c r="N114" t="n">
-        <v>24297.1291</v>
+        <v>11744.82753</v>
       </c>
       <c r="O114" t="n">
-        <v>2094.514016</v>
+        <v>1054.587848</v>
       </c>
       <c r="P114" t="n">
-        <v>0.2468110338</v>
+        <v>0.3108179994</v>
       </c>
       <c r="Q114" t="n">
-        <v>2811.446163</v>
+        <v>1761.484577</v>
       </c>
       <c r="R114" t="n">
-        <v>5026.394183</v>
+        <v>1997.275881</v>
       </c>
       <c r="S114" t="n">
-        <v>19.26523705</v>
+        <v>18.58193867</v>
       </c>
       <c r="T114" t="n">
-        <v>0.355147915</v>
+        <v>0.6439693033</v>
       </c>
       <c r="U114" t="n">
-        <v>3.748662473</v>
+        <v>86.26648196</v>
       </c>
       <c r="V114" t="n">
-        <v>0.4064168635</v>
+        <v>0.3568195952</v>
       </c>
       <c r="W114" t="n">
-        <v>6.462244737</v>
+        <v>5.747833919</v>
       </c>
       <c r="X114" t="n">
-        <v>0.3592340736</v>
+        <v>0.1431272272</v>
       </c>
       <c r="Y114" t="n">
-        <v>3.170700886</v>
+        <v>1.904523708</v>
       </c>
       <c r="Z114" t="n">
-        <v>0.3592340736</v>
+        <v>0.1431272272</v>
       </c>
       <c r="AA114" t="n">
-        <v>2.096219056</v>
+        <v>1.028396768</v>
       </c>
       <c r="AB114" t="n">
-        <v>2.874785825</v>
+        <v>1.794905453</v>
       </c>
       <c r="AC114" t="n">
-        <v>0.2959150605</v>
+        <v>0.1096182547</v>
       </c>
       <c r="AD114" t="n">
-        <v>10041.36129</v>
+        <v>4574.695803</v>
       </c>
       <c r="AE114" t="n">
-        <v>2366.974815</v>
+        <v>1844.601996</v>
       </c>
       <c r="AF114" t="n">
-        <v>2085.366131</v>
+        <v>2808.576567</v>
       </c>
       <c r="AG114" t="n">
-        <v>35.5147915</v>
+        <v>64.39693033</v>
       </c>
       <c r="AH114" t="n">
-        <v>179.9863113</v>
+        <v>90.01411802</v>
       </c>
       <c r="AI114" t="n">
-        <v>89.98741384</v>
+        <v>179.982886</v>
       </c>
       <c r="AJ114" t="n">
-        <v>116.4894444</v>
+        <v>47.75822644</v>
       </c>
       <c r="AK114" t="n">
-        <v>66.7365106</v>
+        <v>85.01997388</v>
       </c>
       <c r="AL114" t="n">
-        <v>0.002411106556</v>
+        <v>0.0002618287306</v>
       </c>
       <c r="AM114" t="n">
-        <v>0.01867745639</v>
+        <v>0.01772906667</v>
       </c>
       <c r="AN114" t="n">
-        <v>8.324575653</v>
+        <v>9.336160755</v>
       </c>
       <c r="AO114" t="n">
-        <v>64.96481084</v>
+        <v>5.309925901</v>
       </c>
       <c r="AP114" t="n">
-        <v>0.3695413995</v>
+        <v>0.4242219987</v>
       </c>
       <c r="AQ114" t="n">
-        <v>1.27374542</v>
+        <v>0.5239727725</v>
       </c>
     </row>
     <row r="115">
@@ -16282,105 +16278,109 @@
         <v>289</v>
       </c>
       <c r="I115" t="n">
-        <v>3675.907948</v>
+        <v>1483.479046</v>
       </c>
       <c r="J115" t="n">
-        <v>0.4458302138</v>
+        <v>0.7797087446</v>
       </c>
       <c r="K115" t="n">
-        <v>5.416227563</v>
+        <v>3.787267596</v>
       </c>
       <c r="L115" t="n">
-        <v>19024.2042</v>
+        <v>6075.941416</v>
       </c>
       <c r="M115" t="n">
-        <v>11105.34999</v>
+        <v>3337.897344</v>
       </c>
       <c r="N115" t="n">
-        <v>30129.55419</v>
+        <v>9413.83876</v>
       </c>
       <c r="O115" t="n">
-        <v>2768.911385</v>
+        <v>1149.312907</v>
       </c>
       <c r="P115" t="n">
-        <v>0.1150687566</v>
+        <v>0.3806497105</v>
       </c>
       <c r="Q115" t="n">
-        <v>3917.940129</v>
+        <v>2039.763261</v>
       </c>
       <c r="R115" t="n">
-        <v>7702.332978</v>
+        <v>2201.453459</v>
       </c>
       <c r="S115" t="n">
-        <v>21.4913624</v>
-      </c>
-      <c r="T115"/>
+        <v>14.16860995</v>
+      </c>
+      <c r="T115" t="n">
+        <v>0.6617627196</v>
+      </c>
       <c r="U115" t="n">
-        <v>3.008000549</v>
+        <v>122.2456505</v>
       </c>
       <c r="V115" t="n">
-        <v>0.4816488332</v>
+        <v>0.4309968176</v>
       </c>
       <c r="W115" t="n">
-        <v>8.218761286</v>
+        <v>8.265669706</v>
       </c>
       <c r="X115" t="n">
-        <v>0.2754560959</v>
+        <v>0.1035935444</v>
       </c>
       <c r="Y115" t="n">
-        <v>4.193461853</v>
+        <v>2.143362705</v>
       </c>
       <c r="Z115" t="n">
-        <v>0.2754560959</v>
+        <v>0.1035935444</v>
       </c>
       <c r="AA115" t="n">
-        <v>2.969420769</v>
+        <v>1.247811042</v>
       </c>
       <c r="AB115" t="n">
-        <v>3.764674437</v>
+        <v>2.028344254</v>
       </c>
       <c r="AC115" t="n">
-        <v>0.4287874157</v>
+        <v>0.1150184513</v>
       </c>
       <c r="AD115" t="n">
-        <v>13329.50195</v>
+        <v>5468.075034</v>
       </c>
       <c r="AE115" t="n">
-        <v>2570.28516</v>
+        <v>2217.368439</v>
       </c>
       <c r="AF115" t="n">
-        <v>2174.670181</v>
-      </c>
-      <c r="AG115"/>
+        <v>2663.497342</v>
+      </c>
+      <c r="AG115" t="n">
+        <v>66.17627196</v>
+      </c>
       <c r="AH115" t="n">
-        <v>179.9912455</v>
+        <v>0.001679790303</v>
       </c>
       <c r="AI115" t="n">
-        <v>90.00696391</v>
+        <v>131.766172</v>
       </c>
       <c r="AJ115" t="n">
-        <v>45.28680563</v>
+        <v>90.00850294</v>
       </c>
       <c r="AK115" t="n">
-        <v>28.96221452</v>
+        <v>73.40629898</v>
       </c>
       <c r="AL115" t="n">
-        <v>0.003448025455</v>
+        <v>0.0008981224234</v>
       </c>
       <c r="AM115" t="n">
-        <v>0.01911123808</v>
+        <v>0.01793588068</v>
       </c>
       <c r="AN115" t="n">
-        <v>10.31765592</v>
+        <v>13.60444702</v>
       </c>
       <c r="AO115" t="n">
-        <v>37.03666524</v>
+        <v>6.374916584</v>
       </c>
       <c r="AP115" t="n">
-        <v>0.4782154096</v>
+        <v>0.1333225378</v>
       </c>
       <c r="AQ115" t="n">
-        <v>1.255825689</v>
+        <v>0.3156375152</v>
       </c>
     </row>
     <row r="116">

</xml_diff>